<commit_message>
[merge] : back-develop <- S07P22D110-59/feature/recommendation/get
</commit_message>
<xml_diff>
--- a/back/demo/src/main/resources/data/location.xlsx
+++ b/back/demo/src/main/resources/data/location.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1000" uniqueCount="458">
   <si>
     <t>Chuncheon-si</t>
   </si>
@@ -194,15 +194,9 @@
     <t>Manan-gu, Anyang-si</t>
   </si>
   <si>
-    <t>안양시만안구</t>
-  </si>
-  <si>
     <t>Dongan-gu, Anyang-si</t>
   </si>
   <si>
-    <t>안양시동안구</t>
-  </si>
-  <si>
     <t>Bucheon-si</t>
   </si>
   <si>
@@ -230,33 +224,18 @@
     <t>Sangnok-gu, Ansan-si</t>
   </si>
   <si>
-    <t>안산시상록구</t>
-  </si>
-  <si>
     <t>Danwon-gu, Ansan-si</t>
   </si>
   <si>
-    <t>안산시단원구</t>
-  </si>
-  <si>
     <t>Deogyang-gu, Goyang-si</t>
   </si>
   <si>
-    <t>고양시덕양구</t>
-  </si>
-  <si>
     <t>Ilsandong-gu, Goyang-si</t>
   </si>
   <si>
-    <t>고양시일산동구</t>
-  </si>
-  <si>
     <t>Ilsanseo-gu, Goyang-si</t>
   </si>
   <si>
-    <t>고양시일산서구</t>
-  </si>
-  <si>
     <t>Gwacheon-si</t>
   </si>
   <si>
@@ -308,9 +287,6 @@
     <t>Cheoin-gu, Yongin-si</t>
   </si>
   <si>
-    <t>용인시처인구</t>
-  </si>
-  <si>
     <t>Giheung-gu, Yongin-si</t>
   </si>
   <si>
@@ -1124,15 +1100,9 @@
     <t>Wansan-gu, Jeonju-si</t>
   </si>
   <si>
-    <t>전주시완산구</t>
-  </si>
-  <si>
     <t>Deokjin-gu, Jeonju-si</t>
   </si>
   <si>
-    <t>전주시덕진구</t>
-  </si>
-  <si>
     <t>Gunsan-si</t>
   </si>
   <si>
@@ -1226,15 +1196,9 @@
     <t>Dongnam-gu, Cheonan-si</t>
   </si>
   <si>
-    <t>천안시동남구</t>
-  </si>
-  <si>
     <t>Seobuk-gu, Cheonan-si</t>
   </si>
   <si>
-    <t>천안시서북구</t>
-  </si>
-  <si>
     <t>Gongju-si</t>
   </si>
   <si>
@@ -1401,6 +1365,62 @@
   </si>
   <si>
     <t>단양군</t>
+  </si>
+  <si>
+    <t>안산시 상록구</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>안산시 단원구</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>고양시 덕양구</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>고양시 일산동구</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>고양시 일산서구</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>안양시 동안구</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>안양시 만안구</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>천안시 동남구</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>천안시 서북구</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전주시 완산구</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전주시 덕진구</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>용인시 처인구</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>용인시 기흥구</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>용인시 수지구</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1784,8 +1804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E250"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="C105" sqref="C105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1801,10 +1821,10 @@
         <v>11110</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="D1" s="1">
         <v>126.977321294872</v>
@@ -1818,10 +1838,10 @@
         <v>11140</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="D2" s="1">
         <v>126.995968139707</v>
@@ -1835,10 +1855,10 @@
         <v>11170</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="D3" s="1">
         <v>126.979906988235</v>
@@ -1852,10 +1872,10 @@
         <v>11200</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="D4" s="1">
         <v>127.04105853332101</v>
@@ -1869,10 +1889,10 @@
         <v>11215</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="D5" s="1">
         <v>127.085744097681</v>
@@ -1886,10 +1906,10 @@
         <v>11230</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="D6" s="1">
         <v>127.05484812780701</v>
@@ -1903,10 +1923,10 @@
         <v>11260</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="D7" s="1">
         <v>127.092883176298</v>
@@ -1920,10 +1940,10 @@
         <v>11290</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="D8" s="1">
         <v>127.01757949116799</v>
@@ -1937,10 +1957,10 @@
         <v>11305</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="D9" s="1">
         <v>127.01118897523899</v>
@@ -1954,10 +1974,10 @@
         <v>11320</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="D10" s="1">
         <v>127.032368819558</v>
@@ -1971,10 +1991,10 @@
         <v>11350</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="D11" s="1">
         <v>127.075034689337</v>
@@ -1988,10 +2008,10 @@
         <v>11380</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="D12" s="1">
         <v>126.92702287719899</v>
@@ -2005,10 +2025,10 @@
         <v>11410</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="D13" s="1">
         <v>126.939063095715</v>
@@ -2022,10 +2042,10 @@
         <v>11440</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="D14" s="1">
         <v>126.90827002744901</v>
@@ -2039,10 +2059,10 @@
         <v>11470</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="D15" s="1">
         <v>126.855477660234</v>
@@ -2056,10 +2076,10 @@
         <v>11500</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="D16" s="1">
         <v>126.822806689705</v>
@@ -2073,10 +2093,10 @@
         <v>11530</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="D17" s="1">
         <v>126.856300578972</v>
@@ -2090,10 +2110,10 @@
         <v>11545</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="D18" s="1">
         <v>126.900820244409</v>
@@ -2107,10 +2127,10 @@
         <v>11560</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="D19" s="1">
         <v>126.91016946737599</v>
@@ -2124,10 +2144,10 @@
         <v>11590</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="D20" s="1">
         <v>126.95164145438299</v>
@@ -2141,10 +2161,10 @@
         <v>11620</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="D21" s="1">
         <v>126.94533715305</v>
@@ -2158,10 +2178,10 @@
         <v>11650</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="D22" s="1">
         <v>127.031220311114</v>
@@ -2175,10 +2195,10 @@
         <v>11680</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="D23" s="1">
         <v>127.062985204247</v>
@@ -2192,10 +2212,10 @@
         <v>11710</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="D24" s="1">
         <v>127.11529503972299</v>
@@ -2209,10 +2229,10 @@
         <v>11740</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="D25" s="1">
         <v>127.14701184176501</v>
@@ -2226,10 +2246,10 @@
         <v>26110</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="D26" s="1">
         <v>129.031540159228</v>
@@ -2243,10 +2263,10 @@
         <v>26140</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="D27" s="1">
         <v>129.014913262627</v>
@@ -2260,10 +2280,10 @@
         <v>26170</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="D28" s="1">
         <v>129.04458557911099</v>
@@ -2277,10 +2297,10 @@
         <v>26200</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="D29" s="1">
         <v>129.06482328776599</v>
@@ -2294,10 +2314,10 @@
         <v>26230</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="D30" s="1">
         <v>129.04306034096101</v>
@@ -2311,10 +2331,10 @@
         <v>26260</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="D31" s="1">
         <v>129.079220086997</v>
@@ -2328,10 +2348,10 @@
         <v>26290</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="D32" s="1">
         <v>129.09400637421001</v>
@@ -2345,10 +2365,10 @@
         <v>26320</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="D33" s="1">
         <v>129.02346325575601</v>
@@ -2362,10 +2382,10 @@
         <v>26350</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="D34" s="1">
         <v>129.15358998958499</v>
@@ -2379,10 +2399,10 @@
         <v>26380</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="D35" s="1">
         <v>128.97380766524299</v>
@@ -2396,10 +2416,10 @@
         <v>26410</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="D36" s="1">
         <v>129.09152874435</v>
@@ -2413,10 +2433,10 @@
         <v>26440</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="D37" s="1">
         <v>128.89240063276199</v>
@@ -2430,10 +2450,10 @@
         <v>26470</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="D38" s="1">
         <v>129.08293526714701</v>
@@ -2447,10 +2467,10 @@
         <v>26500</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="D39" s="1">
         <v>129.111162702944</v>
@@ -2464,10 +2484,10 @@
         <v>26530</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="D40" s="1">
         <v>128.98659237355</v>
@@ -2481,10 +2501,10 @@
         <v>26710</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="D41" s="1">
         <v>129.20095599307999</v>
@@ -2498,10 +2518,10 @@
         <v>27110</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="D42" s="1">
         <v>128.593605829897</v>
@@ -2515,10 +2535,10 @@
         <v>27140</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="D43" s="1">
         <v>128.68565991987799</v>
@@ -2532,10 +2552,10 @@
         <v>27170</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="D44" s="1">
         <v>128.54969760013799</v>
@@ -2549,10 +2569,10 @@
         <v>27200</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="D45" s="1">
         <v>128.58532962764701</v>
@@ -2566,10 +2586,10 @@
         <v>27230</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="D46" s="1">
         <v>128.577204365928</v>
@@ -2583,10 +2603,10 @@
         <v>27260</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="D47" s="1">
         <v>128.66127441262</v>
@@ -2600,10 +2620,10 @@
         <v>27290</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="D48" s="1">
         <v>128.52921214045199</v>
@@ -2617,10 +2637,10 @@
         <v>27710</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="D49" s="1">
         <v>128.49829809573501</v>
@@ -2634,10 +2654,10 @@
         <v>28110</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="D50" s="1">
         <v>126.48283750624699</v>
@@ -2651,10 +2671,10 @@
         <v>28140</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="D51" s="1">
         <v>126.63954391791999</v>
@@ -2668,10 +2688,10 @@
         <v>28177</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="D52" s="1">
         <v>126.66465739133599</v>
@@ -2685,10 +2705,10 @@
         <v>28185</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="D53" s="1">
         <v>126.64883462634801</v>
@@ -2702,10 +2722,10 @@
         <v>28200</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="D54" s="1">
         <v>126.726459491784</v>
@@ -2719,10 +2739,10 @@
         <v>28237</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="D55" s="1">
         <v>126.72120944765</v>
@@ -2736,10 +2756,10 @@
         <v>28245</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="D56" s="1">
         <v>126.734699930007</v>
@@ -2753,10 +2773,10 @@
         <v>28260</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="D57" s="1">
         <v>126.65636443959799</v>
@@ -2770,10 +2790,10 @@
         <v>28710</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="D58" s="1">
         <v>126.40208536016</v>
@@ -2787,10 +2807,10 @@
         <v>28720</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="D59" s="1">
         <v>125.635990786604</v>
@@ -2804,10 +2824,10 @@
         <v>29110</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="D60" s="1">
         <v>126.949464278292</v>
@@ -2821,10 +2841,10 @@
         <v>29140</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="D61" s="1">
         <v>126.85071913996499</v>
@@ -2838,10 +2858,10 @@
         <v>29155</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="D62" s="1">
         <v>126.856718099182</v>
@@ -2855,10 +2875,10 @@
         <v>29170</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="D63" s="1">
         <v>126.925486478595</v>
@@ -2872,10 +2892,10 @@
         <v>29200</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="D64" s="1">
         <v>126.752895215221</v>
@@ -2889,10 +2909,10 @@
         <v>30110</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="D65" s="1">
         <v>127.47503742681801</v>
@@ -2906,10 +2926,10 @@
         <v>30140</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="D66" s="1">
         <v>127.411057308425</v>
@@ -2923,10 +2943,10 @@
         <v>30170</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="D67" s="1">
         <v>127.34510412515699</v>
@@ -2940,10 +2960,10 @@
         <v>30200</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="D68" s="1">
         <v>127.333256401426</v>
@@ -2957,10 +2977,10 @@
         <v>30230</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="D69" s="1">
         <v>127.44015180936</v>
@@ -2974,10 +2994,10 @@
         <v>31110</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="D70" s="1">
         <v>129.30824285432701</v>
@@ -2991,10 +3011,10 @@
         <v>31140</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="D71" s="1">
         <v>129.32820225903899</v>
@@ -3008,10 +3028,10 @@
         <v>31170</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="D72" s="1">
         <v>129.42606551516599</v>
@@ -3025,10 +3045,10 @@
         <v>31200</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="D73" s="1">
         <v>129.37981050604699</v>
@@ -3042,10 +3062,10 @@
         <v>31710</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="D74" s="1">
         <v>129.18692549830701</v>
@@ -3059,10 +3079,10 @@
         <v>36110</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="D75" s="1">
         <v>127.25878005171</v>
@@ -3215,7 +3235,7 @@
         <v>52</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>53</v>
+        <v>450</v>
       </c>
       <c r="D84" s="1">
         <v>126.911385562953</v>
@@ -3229,10 +3249,10 @@
         <v>41173</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>55</v>
+        <v>449</v>
       </c>
       <c r="D85" s="1">
         <v>126.955502710589</v>
@@ -3246,10 +3266,10 @@
         <v>41190</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D86" s="1">
         <v>126.788710884832</v>
@@ -3263,10 +3283,10 @@
         <v>41210</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D87" s="1">
         <v>126.864701314374</v>
@@ -3280,10 +3300,10 @@
         <v>41220</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D88" s="1">
         <v>126.98770073111601</v>
@@ -3297,10 +3317,10 @@
         <v>41250</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D89" s="1">
         <v>127.077912731502</v>
@@ -3314,10 +3334,10 @@
         <v>41271</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>65</v>
+        <v>444</v>
       </c>
       <c r="D90" s="1">
         <v>126.87081503514899</v>
@@ -3331,10 +3351,10 @@
         <v>41273</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>67</v>
+        <v>445</v>
       </c>
       <c r="D91" s="1">
         <v>126.694041180178</v>
@@ -3348,10 +3368,10 @@
         <v>41281</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>69</v>
+        <v>446</v>
       </c>
       <c r="D92" s="1">
         <v>126.87863210137699</v>
@@ -3365,10 +3385,10 @@
         <v>41285</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>71</v>
+        <v>447</v>
       </c>
       <c r="D93" s="1">
         <v>126.79755818288901</v>
@@ -3382,10 +3402,10 @@
         <v>41287</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>73</v>
+        <v>448</v>
       </c>
       <c r="D94" s="1">
         <v>126.727983527863</v>
@@ -3399,10 +3419,10 @@
         <v>41290</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="D95" s="1">
         <v>127.002679466968</v>
@@ -3416,10 +3436,10 @@
         <v>41310</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="D96" s="1">
         <v>127.13122991777701</v>
@@ -3433,10 +3453,10 @@
         <v>41360</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D97" s="1">
         <v>127.24366064477999</v>
@@ -3450,10 +3470,10 @@
         <v>41370</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="D98" s="1">
         <v>127.051329667291</v>
@@ -3467,10 +3487,10 @@
         <v>41390</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="D99" s="1">
         <v>126.78839282675099</v>
@@ -3484,10 +3504,10 @@
         <v>41410</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="D100" s="1">
         <v>126.92113468846399</v>
@@ -3501,10 +3521,10 @@
         <v>41430</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D101" s="1">
         <v>126.989625456095</v>
@@ -3518,10 +3538,10 @@
         <v>41450</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D102" s="1">
         <v>127.20594379921</v>
@@ -3535,10 +3555,10 @@
         <v>41461</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>91</v>
+        <v>455</v>
       </c>
       <c r="D103" s="1">
         <v>127.252933149866</v>
@@ -3552,10 +3572,10 @@
         <v>41463</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>93</v>
+        <v>456</v>
       </c>
       <c r="D104" s="1">
         <v>127.121340845942</v>
@@ -3569,10 +3589,10 @@
         <v>41465</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>95</v>
+        <v>457</v>
       </c>
       <c r="D105" s="1">
         <v>127.071551073175</v>
@@ -3586,10 +3606,10 @@
         <v>41480</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="D106" s="1">
         <v>126.81063317186</v>
@@ -3603,10 +3623,10 @@
         <v>41500</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="D107" s="1">
         <v>127.481014112008</v>
@@ -3620,10 +3640,10 @@
         <v>41550</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="D108" s="1">
         <v>127.302722292128</v>
@@ -3637,10 +3657,10 @@
         <v>41570</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="D109" s="1">
         <v>126.62643062238701</v>
@@ -3654,10 +3674,10 @@
         <v>41590</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="D110" s="1">
         <v>126.874858719182</v>
@@ -3671,10 +3691,10 @@
         <v>41610</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="D111" s="1">
         <v>127.30117595196</v>
@@ -3688,10 +3708,10 @@
         <v>41630</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="D112" s="1">
         <v>127.001134902898</v>
@@ -3705,10 +3725,10 @@
         <v>41650</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="D113" s="1">
         <v>127.250337280304</v>
@@ -3722,10 +3742,10 @@
         <v>41670</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="D114" s="1">
         <v>127.615737344978</v>
@@ -3739,10 +3759,10 @@
         <v>41800</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="D115" s="1">
         <v>127.024456396852</v>
@@ -3756,10 +3776,10 @@
         <v>41820</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="D116" s="1">
         <v>127.450192131089</v>
@@ -3773,10 +3793,10 @@
         <v>41830</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="D117" s="1">
         <v>127.579264460353</v>
@@ -4096,10 +4116,10 @@
         <v>43111</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>428</v>
+        <v>416</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>429</v>
+        <v>417</v>
       </c>
       <c r="D136" s="1">
         <v>127.584881845482</v>
@@ -4113,10 +4133,10 @@
         <v>43112</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>430</v>
+        <v>418</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>431</v>
+        <v>419</v>
       </c>
       <c r="D137" s="1">
         <v>127.43840329587</v>
@@ -4130,10 +4150,10 @@
         <v>43113</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>432</v>
+        <v>420</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>433</v>
+        <v>421</v>
       </c>
       <c r="D138" s="1">
         <v>127.36927488397301</v>
@@ -4147,10 +4167,10 @@
         <v>43114</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>434</v>
+        <v>422</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>435</v>
+        <v>423</v>
       </c>
       <c r="D139" s="1">
         <v>127.491317617216</v>
@@ -4164,10 +4184,10 @@
         <v>43130</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>436</v>
+        <v>424</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>437</v>
+        <v>425</v>
       </c>
       <c r="D140" s="1">
         <v>127.895662264793</v>
@@ -4181,10 +4201,10 @@
         <v>43150</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>438</v>
+        <v>426</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>439</v>
+        <v>427</v>
       </c>
       <c r="D141" s="1">
         <v>128.140959298263</v>
@@ -4198,10 +4218,10 @@
         <v>43720</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>440</v>
+        <v>428</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="D142" s="1">
         <v>127.729335671527</v>
@@ -4215,10 +4235,10 @@
         <v>43730</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>442</v>
+        <v>430</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>443</v>
+        <v>431</v>
       </c>
       <c r="D143" s="1">
         <v>127.656558857677</v>
@@ -4232,10 +4252,10 @@
         <v>43740</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>444</v>
+        <v>432</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>445</v>
+        <v>433</v>
       </c>
       <c r="D144" s="1">
         <v>127.814228143628</v>
@@ -4249,10 +4269,10 @@
         <v>43745</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>446</v>
+        <v>434</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>447</v>
+        <v>435</v>
       </c>
       <c r="D145" s="1">
         <v>127.60461807823199</v>
@@ -4266,10 +4286,10 @@
         <v>43750</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>448</v>
+        <v>436</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>449</v>
+        <v>437</v>
       </c>
       <c r="D146" s="1">
         <v>127.440463550866</v>
@@ -4283,10 +4303,10 @@
         <v>43760</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>451</v>
+        <v>439</v>
       </c>
       <c r="D147" s="1">
         <v>127.829588124542</v>
@@ -4300,10 +4320,10 @@
         <v>43770</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>452</v>
+        <v>440</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>453</v>
+        <v>441</v>
       </c>
       <c r="D148" s="1">
         <v>127.614206769649</v>
@@ -4317,10 +4337,10 @@
         <v>43800</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>454</v>
+        <v>442</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>455</v>
+        <v>443</v>
       </c>
       <c r="D149" s="1">
         <v>128.38784162081001</v>
@@ -4334,10 +4354,10 @@
         <v>44131</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>396</v>
+        <v>386</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>397</v>
+        <v>451</v>
       </c>
       <c r="D150" s="1">
         <v>127.220894604506</v>
@@ -4351,10 +4371,10 @@
         <v>44133</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>398</v>
+        <v>387</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>399</v>
+        <v>452</v>
       </c>
       <c r="D151" s="1">
         <v>127.16180940387</v>
@@ -4368,10 +4388,10 @@
         <v>44150</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>400</v>
+        <v>388</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>401</v>
+        <v>389</v>
       </c>
       <c r="D152" s="1">
         <v>127.07521911409199</v>
@@ -4385,10 +4405,10 @@
         <v>44180</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>402</v>
+        <v>390</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>403</v>
+        <v>391</v>
       </c>
       <c r="D153" s="1">
         <v>126.592969076198</v>
@@ -4402,10 +4422,10 @@
         <v>44200</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>404</v>
+        <v>392</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>405</v>
+        <v>393</v>
       </c>
       <c r="D154" s="1">
         <v>126.98007557008199</v>
@@ -4419,10 +4439,10 @@
         <v>44210</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>406</v>
+        <v>394</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>407</v>
+        <v>395</v>
       </c>
       <c r="D155" s="1">
         <v>126.46360158405</v>
@@ -4436,10 +4456,10 @@
         <v>44230</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>408</v>
+        <v>396</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>409</v>
+        <v>397</v>
       </c>
       <c r="D156" s="1">
         <v>127.157716376655</v>
@@ -4453,10 +4473,10 @@
         <v>44250</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>410</v>
+        <v>398</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>411</v>
+        <v>399</v>
       </c>
       <c r="D157" s="1">
         <v>127.234426611849</v>
@@ -4470,10 +4490,10 @@
         <v>44270</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>412</v>
+        <v>400</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>413</v>
+        <v>401</v>
       </c>
       <c r="D158" s="1">
         <v>126.652744489844</v>
@@ -4487,10 +4507,10 @@
         <v>44710</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>414</v>
+        <v>402</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>415</v>
+        <v>403</v>
       </c>
       <c r="D159" s="1">
         <v>127.47831188873199</v>
@@ -4504,10 +4524,10 @@
         <v>44760</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>416</v>
+        <v>404</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>417</v>
+        <v>405</v>
       </c>
       <c r="D160" s="1">
         <v>126.856967641628</v>
@@ -4521,10 +4541,10 @@
         <v>44770</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>418</v>
+        <v>406</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>419</v>
+        <v>407</v>
       </c>
       <c r="D161" s="1">
         <v>126.704956417305</v>
@@ -4538,10 +4558,10 @@
         <v>44790</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>420</v>
+        <v>408</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>421</v>
+        <v>409</v>
       </c>
       <c r="D162" s="1">
         <v>126.85311311134799</v>
@@ -4555,10 +4575,10 @@
         <v>44800</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>422</v>
+        <v>410</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>423</v>
+        <v>411</v>
       </c>
       <c r="D163" s="1">
         <v>126.62582959709501</v>
@@ -4572,10 +4592,10 @@
         <v>44810</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>424</v>
+        <v>412</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>425</v>
+        <v>413</v>
       </c>
       <c r="D164" s="1">
         <v>126.784309990144</v>
@@ -4589,10 +4609,10 @@
         <v>44825</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>426</v>
+        <v>414</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>427</v>
+        <v>415</v>
       </c>
       <c r="D165" s="1">
         <v>126.28095711045501</v>
@@ -4606,10 +4626,10 @@
         <v>45111</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>363</v>
+        <v>453</v>
       </c>
       <c r="D166" s="1">
         <v>127.120764418251</v>
@@ -4623,10 +4643,10 @@
         <v>45113</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>364</v>
+        <v>355</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>365</v>
+        <v>454</v>
       </c>
       <c r="D167" s="1">
         <v>127.11175319980801</v>
@@ -4640,10 +4660,10 @@
         <v>45130</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>366</v>
+        <v>356</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="D168" s="1">
         <v>126.726015246248</v>
@@ -4657,10 +4677,10 @@
         <v>45140</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>368</v>
+        <v>358</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>369</v>
+        <v>359</v>
       </c>
       <c r="D169" s="1">
         <v>126.989510169826</v>
@@ -4674,10 +4694,10 @@
         <v>45180</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>370</v>
+        <v>360</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>371</v>
+        <v>361</v>
       </c>
       <c r="D170" s="1">
         <v>126.905857544493</v>
@@ -4691,10 +4711,10 @@
         <v>45190</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>372</v>
+        <v>362</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>373</v>
+        <v>363</v>
       </c>
       <c r="D171" s="1">
         <v>127.441889737369</v>
@@ -4708,10 +4728,10 @@
         <v>45210</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>374</v>
+        <v>364</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>375</v>
+        <v>365</v>
       </c>
       <c r="D172" s="1">
         <v>126.89488569577701</v>
@@ -4725,10 +4745,10 @@
         <v>45710</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>376</v>
+        <v>366</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>377</v>
+        <v>367</v>
       </c>
       <c r="D173" s="1">
         <v>127.215114637507</v>
@@ -4742,10 +4762,10 @@
         <v>45720</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="D174" s="1">
         <v>127.430035441264</v>
@@ -4759,10 +4779,10 @@
         <v>45730</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>380</v>
+        <v>370</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="D175" s="1">
         <v>127.712953110664</v>
@@ -4776,10 +4796,10 @@
         <v>45740</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>382</v>
+        <v>372</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>383</v>
+        <v>373</v>
       </c>
       <c r="D176" s="1">
         <v>127.544264073338</v>
@@ -4793,10 +4813,10 @@
         <v>45750</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>384</v>
+        <v>374</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>385</v>
+        <v>375</v>
       </c>
       <c r="D177" s="1">
         <v>127.23664715076001</v>
@@ -4810,10 +4830,10 @@
         <v>45770</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>386</v>
+        <v>376</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>387</v>
+        <v>377</v>
       </c>
       <c r="D178" s="1">
         <v>127.090086973909</v>
@@ -4827,10 +4847,10 @@
         <v>45790</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>388</v>
+        <v>378</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="D179" s="1">
         <v>126.61604618382</v>
@@ -4844,10 +4864,10 @@
         <v>45800</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
       <c r="D180" s="1">
         <v>126.644377397867</v>
@@ -4861,10 +4881,10 @@
         <v>46110</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="D181" s="1">
         <v>126.39183527988401</v>
@@ -4878,10 +4898,10 @@
         <v>46130</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="D182" s="1">
         <v>127.653355313245</v>
@@ -4895,10 +4915,10 @@
         <v>46150</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="D183" s="1">
         <v>127.389162729226</v>
@@ -4912,10 +4932,10 @@
         <v>46170</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="D184" s="1">
         <v>126.72041032044</v>
@@ -4929,10 +4949,10 @@
         <v>46230</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="D185" s="1">
         <v>127.65512791424899</v>
@@ -4946,10 +4966,10 @@
         <v>46710</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="D186" s="1">
         <v>126.99529085588</v>
@@ -4963,10 +4983,10 @@
         <v>46720</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="D187" s="1">
         <v>127.263582521481</v>
@@ -4980,10 +5000,10 @@
         <v>46730</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="D188" s="1">
         <v>127.503119252262</v>
@@ -4997,10 +5017,10 @@
         <v>46770</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="D189" s="1">
         <v>127.314620496808</v>
@@ -5014,10 +5034,10 @@
         <v>46780</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="D190" s="1">
         <v>127.16212135652999</v>
@@ -5031,10 +5051,10 @@
         <v>46790</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="D191" s="1">
         <v>127.03343353596701</v>
@@ -5048,10 +5068,10 @@
         <v>46800</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="D192" s="1">
         <v>126.92153234303299</v>
@@ -5065,10 +5085,10 @@
         <v>46810</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="D193" s="1">
         <v>126.772156286377</v>
@@ -5082,10 +5102,10 @@
         <v>46820</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="D194" s="1">
         <v>126.51171496166501</v>
@@ -5099,10 +5119,10 @@
         <v>46830</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="D195" s="1">
         <v>126.630694486251</v>
@@ -5116,10 +5136,10 @@
         <v>46840</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
       <c r="D196" s="1">
         <v>126.42590789480801</v>
@@ -5133,10 +5153,10 @@
         <v>46860</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>351</v>
+        <v>343</v>
       </c>
       <c r="D197" s="1">
         <v>126.535604073215</v>
@@ -5150,10 +5170,10 @@
         <v>46870</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>352</v>
+        <v>344</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="D198" s="1">
         <v>126.453129290159</v>
@@ -5167,10 +5187,10 @@
         <v>46880</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="D199" s="1">
         <v>126.76849489913501</v>
@@ -5184,10 +5204,10 @@
         <v>46890</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="D200" s="1">
         <v>126.776806856665</v>
@@ -5201,10 +5221,10 @@
         <v>46900</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="D201" s="1">
         <v>126.215057844789</v>
@@ -5218,10 +5238,10 @@
         <v>46910</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="D202" s="1">
         <v>126.04890702742399</v>
@@ -5235,10 +5255,10 @@
         <v>47111</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="D203" s="1">
         <v>129.43761667189401</v>
@@ -5252,10 +5272,10 @@
         <v>47113</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="D204" s="1">
         <v>129.23405313974999</v>
@@ -5269,10 +5289,10 @@
         <v>47130</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C205" s="1" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="D205" s="1">
         <v>129.235929627697</v>
@@ -5286,10 +5306,10 @@
         <v>47150</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="C206" s="1" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="D206" s="1">
         <v>128.077707549124</v>
@@ -5303,10 +5323,10 @@
         <v>47170</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="C207" s="1" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="D207" s="1">
         <v>128.780042683869</v>
@@ -5320,10 +5340,10 @@
         <v>47190</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="C208" s="1" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="D208" s="1">
         <v>128.35555547951401</v>
@@ -5337,10 +5357,10 @@
         <v>47210</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="C209" s="1" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="D209" s="1">
         <v>128.59768261657399</v>
@@ -5354,10 +5374,10 @@
         <v>47230</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="C210" s="1" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="D210" s="1">
         <v>128.94262401550699</v>
@@ -5371,10 +5391,10 @@
         <v>47250</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="D211" s="1">
         <v>128.067007021683</v>
@@ -5388,10 +5408,10 @@
         <v>47280</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="C212" s="1" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="D212" s="1">
         <v>128.14860817477501</v>
@@ -5405,10 +5425,10 @@
         <v>47290</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="C213" s="1" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="D213" s="1">
         <v>128.80905515042599</v>
@@ -5422,10 +5442,10 @@
         <v>47720</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="C214" s="1" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="D214" s="1">
         <v>128.64822460165701</v>
@@ -5439,10 +5459,10 @@
         <v>47730</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="C215" s="1" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="D215" s="1">
         <v>128.61506730951501</v>
@@ -5456,10 +5476,10 @@
         <v>47750</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="C216" s="1" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="D216" s="1">
         <v>129.05738517931101</v>
@@ -5473,10 +5493,10 @@
         <v>47760</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="C217" s="1" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="D217" s="1">
         <v>129.145030452247</v>
@@ -5490,10 +5510,10 @@
         <v>47770</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="C218" s="1" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="D218" s="1">
         <v>129.31737621079699</v>
@@ -5507,10 +5527,10 @@
         <v>47820</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="C219" s="1" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="D219" s="1">
         <v>128.78652700766901</v>
@@ -5524,10 +5544,10 @@
         <v>47830</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="C220" s="1" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D220" s="1">
         <v>128.30673370969799</v>
@@ -5541,10 +5561,10 @@
         <v>47840</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="C221" s="1" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="D221" s="1">
         <v>128.233393081636</v>
@@ -5558,10 +5578,10 @@
         <v>47850</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="C222" s="1" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="D222" s="1">
         <v>128.46258382615099</v>
@@ -5575,10 +5595,10 @@
         <v>47900</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="C223" s="1" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="D223" s="1">
         <v>128.42238404626099</v>
@@ -5592,10 +5612,10 @@
         <v>47920</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="C224" s="1" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="D224" s="1">
         <v>128.91290040087301</v>
@@ -5609,10 +5629,10 @@
         <v>47930</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="C225" s="1" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="D225" s="1">
         <v>129.31231855913401</v>
@@ -5626,10 +5646,10 @@
         <v>47940</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="C226" s="1" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="D226" s="1">
         <v>130.864188011946</v>
@@ -5643,10 +5663,10 @@
         <v>48121</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="C227" s="1" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="D227" s="1">
         <v>128.649555126064</v>
@@ -5660,10 +5680,10 @@
         <v>48123</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="C228" s="1" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="D228" s="1">
         <v>128.672073660796</v>
@@ -5677,10 +5697,10 @@
         <v>48125</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="C229" s="1" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="D229" s="1">
         <v>128.485255846076</v>
@@ -5694,10 +5714,10 @@
         <v>48127</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="C230" s="1" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="D230" s="1">
         <v>128.53643316420801</v>
@@ -5711,10 +5731,10 @@
         <v>48129</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C231" s="1" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="D231" s="1">
         <v>128.73630082645201</v>
@@ -5728,10 +5748,10 @@
         <v>48170</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="C232" s="1" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="D232" s="1">
         <v>128.12980113082699</v>
@@ -5745,10 +5765,10 @@
         <v>48220</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C233" s="1" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="D233" s="1">
         <v>128.374075369107</v>
@@ -5762,10 +5782,10 @@
         <v>48240</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="C234" s="1" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="D234" s="1">
         <v>128.03769634830601</v>
@@ -5779,10 +5799,10 @@
         <v>48250</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="C235" s="1" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="D235" s="1">
         <v>128.845215755417</v>
@@ -5796,10 +5816,10 @@
         <v>48270</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="C236" s="1" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="D236" s="1">
         <v>128.789601450872</v>
@@ -5813,10 +5833,10 @@
         <v>48310</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="C237" s="1" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="D237" s="1">
         <v>128.623135098848</v>
@@ -5830,10 +5850,10 @@
         <v>48330</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="C238" s="1" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="D238" s="1">
         <v>129.04104144169199</v>
@@ -5847,10 +5867,10 @@
         <v>48720</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="C239" s="1" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="D239" s="1">
         <v>128.277057796641</v>
@@ -5864,10 +5884,10 @@
         <v>48730</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="C240" s="1" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="D240" s="1">
         <v>128.430876889514</v>
@@ -5881,10 +5901,10 @@
         <v>48740</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="C241" s="1" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="D241" s="1">
         <v>128.49305192575099</v>
@@ -5915,10 +5935,10 @@
         <v>48840</v>
       </c>
       <c r="B243" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="C243" s="1" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="D243" s="1">
         <v>127.94114052543</v>
@@ -5932,10 +5952,10 @@
         <v>48850</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="C244" s="1" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="D244" s="1">
         <v>127.779049000006</v>
@@ -5949,10 +5969,10 @@
         <v>48860</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="C245" s="1" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="D245" s="1">
         <v>127.88433791961199</v>
@@ -5966,10 +5986,10 @@
         <v>48870</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="C246" s="1" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D246" s="1">
         <v>127.72204105707701</v>
@@ -5983,10 +6003,10 @@
         <v>48880</v>
       </c>
       <c r="B247" s="1" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="C247" s="1" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="D247" s="1">
         <v>127.90416955131001</v>
@@ -6000,10 +6020,10 @@
         <v>48890</v>
       </c>
       <c r="B248" s="1" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C248" s="1" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="D248" s="1">
         <v>128.141543703888</v>
@@ -6017,10 +6037,10 @@
         <v>50110</v>
       </c>
       <c r="B249" s="1" t="s">
-        <v>392</v>
+        <v>382</v>
       </c>
       <c r="C249" s="1" t="s">
-        <v>393</v>
+        <v>383</v>
       </c>
       <c r="D249" s="1">
         <v>126.529247612329</v>
@@ -6034,10 +6054,10 @@
         <v>50130</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>394</v>
+        <v>384</v>
       </c>
       <c r="C250" s="1" t="s">
-        <v>395</v>
+        <v>385</v>
       </c>
       <c r="D250" s="1">
         <v>126.581085738056</v>
@@ -6049,5 +6069,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>